<commit_message>
Changed logic of OutPutService
</commit_message>
<xml_diff>
--- a/Warehouse/Resources/Card.xlsx
+++ b/Warehouse/Resources/Card.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Карточка складского учёта</t>
   </si>
@@ -33,6 +33,9 @@
     <t>ОАО Гомельский Мясокомбинат</t>
   </si>
   <si>
+    <t>Продукт: Волковыское</t>
+  </si>
+  <si>
     <t>Главный склад</t>
   </si>
   <si>
@@ -48,37 +51,31 @@
     <t>Расход</t>
   </si>
   <si>
-    <t>Магма</t>
+    <t>Остаток</t>
+  </si>
+  <si>
+    <t>Волковыское</t>
+  </si>
+  <si>
+    <t>100</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>249</t>
-  </si>
-  <si>
-    <t>Тесто</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>Новое</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>52</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>124</t>
-  </si>
-  <si>
-    <t>122</t>
+    <t>63</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>177</t>
+  </si>
+  <si>
+    <t>214</t>
+  </si>
+  <si>
+    <t>Составил: _______________</t>
   </si>
 </sst>
 </file>
@@ -125,10 +122,10 @@
   <cellXfs count="5">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1"/>
@@ -412,7 +409,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -421,6 +418,7 @@
     <col min="1" max="1" width="20" customWidth="1" style="1"/>
     <col min="2" max="2" width="20" customWidth="1" style="1"/>
     <col min="3" max="3" width="20" customWidth="1" style="1"/>
+    <col min="4" max="4" width="20" customWidth="1" style="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -433,6 +431,9 @@
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
@@ -444,6 +445,9 @@
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
@@ -455,6 +459,9 @@
       <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
@@ -466,129 +473,93 @@
       <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>6</v>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>8</v>
+      <c r="D8" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>8</v>
+      <c r="D10" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="A12" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
   </mergeCells>
   <pageSetup orientation="landscape"/>
   <headerFooter/>

</xml_diff>